<commit_message>
Update Microcontroller pinout assignments.xlsx
</commit_message>
<xml_diff>
--- a/Microcontroller pinout assignments.xlsx
+++ b/Microcontroller pinout assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2ac6356bae23d48/Documents/^NCODE/SmartCAR/GrabCrab_smartcar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{5A3D812F-B50B-485F-A7E0-E98D5B77DB96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76D7ABDD-86A3-4D9E-9023-A47BF418A7A9}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{5A3D812F-B50B-485F-A7E0-E98D5B77DB96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{21A47187-B929-42CA-93D8-90B1FBFDB306}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{07093BA4-AFBC-41B7-9BBC-A69CB304ADA0}"/>
+    <workbookView xWindow="10530" yWindow="1170" windowWidth="15825" windowHeight="12495" xr2:uid="{07093BA4-AFBC-41B7-9BBC-A69CB304ADA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>TX1</t>
   </si>
@@ -265,13 +265,37 @@
   </si>
   <si>
     <t>RPi : AI, SLAM &amp; controller</t>
+  </si>
+  <si>
+    <t>Arduino Mega Pinout</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>IOREF</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>Vin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +331,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +359,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -355,22 +404,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Beregning" xfId="2" builtinId="22"/>
-    <cellStyle name="Dårlig" xfId="3" builtinId="27"/>
-    <cellStyle name="Inndata" xfId="1" builtinId="20"/>
+  <cellStyles count="7">
+    <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
+    <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,7 +445,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -683,13 +741,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE36539-01AF-4AFE-888C-B5DD988BEFDF}">
-  <dimension ref="B6:Q26"/>
+  <dimension ref="B6:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
@@ -827,7 +885,7 @@
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -857,7 +915,7 @@
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -887,10 +945,10 @@
       <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="1"/>
@@ -915,10 +973,10 @@
       <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="1"/>
@@ -943,10 +1001,10 @@
       <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="1"/>
@@ -971,10 +1029,10 @@
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="1"/>
@@ -999,10 +1057,10 @@
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="1"/>
@@ -1027,10 +1085,10 @@
       <c r="B18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="1"/>
@@ -1055,7 +1113,7 @@
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1083,7 +1141,7 @@
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1111,10 +1169,10 @@
       <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -1178,6 +1236,9 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="2" t="s">
         <v>3</v>
@@ -1186,6 +1247,52 @@
         <v>75</v>
       </c>
       <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>